<commit_message>
Add more cells below the first matrix formula cells.
</commit_message>
<xml_diff>
--- a/test/xlsx/formula-array-1/input.xlsx
+++ b/test/xlsx/formula-array-1/input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\workspace\orcus\test\xlsx\formula-array-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kohei\workspace\orcus\test\xlsx\formula-array-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE6B4D6B-DC40-481B-9757-867C928789BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1573D3-7D93-4E50-9297-38FF19C8B619}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{9F1A5D6E-345D-4E43-B9EF-989A90D405BF}"/>
   </bookViews>
@@ -371,15 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF86C16-8C11-48FD-B870-5B8550F2E456}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -393,17 +393,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5">
         <f t="array" ref="C5:E7">MMULT(A1:A3,C1:E1)</f>
         <v>4</v>
@@ -415,7 +415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>8</v>
       </c>
@@ -426,7 +426,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>12</v>
       </c>
@@ -435,6 +435,35 @@
       </c>
       <c r="E7">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <f t="array" ref="F9:G10">MMULT(A9:A10,C9:D9)</f>
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>40</v>
+      </c>
+      <c r="G10">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>